<commit_message>
Added gui for withdraw and refund for buyer
</commit_message>
<xml_diff>
--- a/results/evaluation.xlsx
+++ b/results/evaluation.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Egon\Desktop\Thesis\confidential-fair-exchange\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFBF83B-1E05-42A2-A8B3-9D02BA9E0E99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C8A5A79-CFE1-439D-879E-8191A1E951E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="-80" windowWidth="21760" windowHeight="13840" activeTab="1" xr2:uid="{5F922745-7528-0F40-B053-CCEE2A7D879C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="21820" windowHeight="13900" activeTab="2" xr2:uid="{5F922745-7528-0F40-B053-CCEE2A7D879C}"/>
   </bookViews>
   <sheets>
     <sheet name="polygon" sheetId="1" r:id="rId1"/>
     <sheet name="ropsten" sheetId="3" r:id="rId2"/>
+    <sheet name="goerli" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="35">
   <si>
     <t>Execution</t>
   </si>
@@ -117,13 +118,37 @@
   </si>
   <si>
     <t>new step diff</t>
+  </si>
+  <si>
+    <t xml:space="preserve">publish file </t>
+  </si>
+  <si>
+    <t>publish desc</t>
+  </si>
+  <si>
+    <t>refundToBuyer</t>
+  </si>
+  <si>
+    <t>FAIRDROP</t>
+  </si>
+  <si>
+    <t>FAIRDEX</t>
+  </si>
+  <si>
+    <t>ADDRESS</t>
+  </si>
+  <si>
+    <t>0x54567cfD53EcA3F0F18D438f084d3a54349Ff131</t>
+  </si>
+  <si>
+    <t>.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -161,6 +186,13 @@
       <sz val="12"/>
       <name val="Consolas"/>
       <family val="3"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF1E2022"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -201,7 +233,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -258,6 +290,20 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -979,8 +1025,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7427C27-8383-400B-9973-D62D6614955F}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="B15:C15"/>
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1242,7 +1288,7 @@
         <v>66125</v>
       </c>
       <c r="E20">
-        <f t="shared" ref="E19:E27" si="0">SUM(B20:D20)</f>
+        <f t="shared" ref="E20:E27" si="0">SUM(B20:D20)</f>
         <v>253514</v>
       </c>
       <c r="F20" s="3"/>
@@ -1465,7 +1511,6 @@
     <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
       <c r="D29" s="3"/>
       <c r="F29" s="3"/>
       <c r="G29" s="3"/>
@@ -1558,7 +1603,7 @@
         <v>57227</v>
       </c>
       <c r="D33" s="14">
-        <f t="shared" si="3"/>
+        <f>INT($D$30+($D$38-$D$30)/8*(A22-$A$19))</f>
         <v>49862</v>
       </c>
       <c r="E33" s="14">
@@ -1900,9 +1945,18 @@
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A51" s="14"/>
-      <c r="B51" s="14"/>
-      <c r="C51" s="14"/>
-      <c r="D51" s="14"/>
+      <c r="B51" s="14">
+        <f>B41/B30*100</f>
+        <v>17.45517792095562</v>
+      </c>
+      <c r="C51" s="14">
+        <f>C41/C30*100</f>
+        <v>39.820364513254233</v>
+      </c>
+      <c r="D51" s="14">
+        <f>D41/D30*100</f>
+        <v>36.024844720496894</v>
+      </c>
       <c r="E51" s="14"/>
       <c r="F51" s="14"/>
       <c r="G51" s="14"/>
@@ -1938,4 +1992,1071 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A7526DE-2927-40F1-9BCF-D315E919FCE8}">
+  <dimension ref="A1:S46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H18" sqref="H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="3" width="14.33203125" customWidth="1"/>
+    <col min="5" max="5" width="8.6640625" customWidth="1"/>
+    <col min="6" max="6" width="14.75" customWidth="1"/>
+    <col min="7" max="7" width="10.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A1" s="21"/>
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
+      <c r="N1" s="21"/>
+      <c r="O1" s="21"/>
+      <c r="P1" s="21"/>
+      <c r="Q1" s="21"/>
+      <c r="R1" s="21"/>
+      <c r="S1" s="21"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A2" s="21"/>
+      <c r="B2" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="C2" s="24"/>
+      <c r="D2" s="21"/>
+      <c r="E2" s="21"/>
+      <c r="F2" s="24" t="s">
+        <v>31</v>
+      </c>
+      <c r="G2" s="24"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
+      <c r="J2" s="21"/>
+      <c r="K2" s="21"/>
+      <c r="L2" s="21"/>
+      <c r="M2" s="21"/>
+      <c r="N2" s="21"/>
+      <c r="O2" s="21"/>
+      <c r="P2" s="21"/>
+      <c r="Q2" s="21"/>
+      <c r="R2" s="21"/>
+      <c r="S2" s="21"/>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A3" s="21"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="24"/>
+      <c r="D3" s="21"/>
+      <c r="E3" s="21"/>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
+      <c r="M3" s="21"/>
+      <c r="N3" s="21"/>
+      <c r="O3" s="21"/>
+      <c r="P3" s="21"/>
+      <c r="Q3" s="21"/>
+      <c r="R3" s="21"/>
+      <c r="S3" s="21"/>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A4" s="21"/>
+      <c r="D4" s="21"/>
+      <c r="E4" s="21"/>
+      <c r="F4" s="21"/>
+      <c r="G4" s="21"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="21"/>
+      <c r="K4" s="21"/>
+      <c r="L4" s="21"/>
+      <c r="M4" s="21"/>
+      <c r="N4" s="21"/>
+      <c r="O4" s="21"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="21"/>
+      <c r="R4" s="21"/>
+      <c r="S4" s="21"/>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A5" s="21"/>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5" s="25" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="E5" s="21"/>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="21"/>
+      <c r="M5" s="21"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="21"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="21"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
+      <c r="K6" s="21"/>
+      <c r="L6" s="21"/>
+      <c r="M6" s="21"/>
+      <c r="N6" s="21"/>
+      <c r="O6" s="21"/>
+      <c r="P6" s="21"/>
+      <c r="Q6" s="21"/>
+      <c r="R6" s="21"/>
+      <c r="S6" s="21"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A7" s="21"/>
+      <c r="B7" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="22">
+        <v>1982723</v>
+      </c>
+      <c r="D7" s="21"/>
+      <c r="E7" s="21"/>
+      <c r="F7" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="G7" s="21"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="21"/>
+      <c r="K7" s="21"/>
+      <c r="L7" s="21"/>
+      <c r="M7" s="21"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="21"/>
+      <c r="P7" s="21"/>
+      <c r="Q7" s="21"/>
+      <c r="R7" s="21"/>
+      <c r="S7" s="21"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A8" s="21"/>
+      <c r="B8" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" s="22">
+        <v>93728</v>
+      </c>
+      <c r="D8" s="21"/>
+      <c r="E8" s="21"/>
+      <c r="F8" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="G8" s="21"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="21"/>
+      <c r="K8" s="21"/>
+      <c r="L8" s="21"/>
+      <c r="M8" s="21"/>
+      <c r="N8" s="21"/>
+      <c r="O8" s="21"/>
+      <c r="P8" s="21"/>
+      <c r="Q8" s="21"/>
+      <c r="R8" s="21"/>
+      <c r="S8" s="21"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A9" s="21"/>
+      <c r="B9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="C9" s="26">
+        <v>48890</v>
+      </c>
+      <c r="D9" s="21"/>
+      <c r="E9" s="21"/>
+      <c r="F9" s="21" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="21"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="21"/>
+      <c r="K9" s="21"/>
+      <c r="L9" s="21"/>
+      <c r="M9" s="21"/>
+      <c r="N9" s="21"/>
+      <c r="O9" s="21"/>
+      <c r="P9" s="21"/>
+      <c r="Q9" s="21"/>
+      <c r="R9" s="21"/>
+      <c r="S9" s="21"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A10" s="21"/>
+      <c r="B10" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="26">
+        <v>107645</v>
+      </c>
+      <c r="D10" s="21"/>
+      <c r="E10" s="21"/>
+      <c r="F10" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="G10" s="21"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="21"/>
+      <c r="K10" s="21"/>
+      <c r="L10" s="21"/>
+      <c r="M10" s="21"/>
+      <c r="N10" s="21"/>
+      <c r="O10" s="21"/>
+      <c r="P10" s="21"/>
+      <c r="Q10" s="21"/>
+      <c r="R10" s="21"/>
+      <c r="S10" s="21"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A11" s="21"/>
+      <c r="B11" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="26">
+        <v>59660</v>
+      </c>
+      <c r="D11" s="21"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="21" t="s">
+        <v>29</v>
+      </c>
+      <c r="G11" s="21"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="21"/>
+      <c r="K11" s="21"/>
+      <c r="L11" s="21"/>
+      <c r="M11" s="21"/>
+      <c r="N11" s="21"/>
+      <c r="O11" s="21"/>
+      <c r="P11" s="21"/>
+      <c r="Q11" s="21"/>
+      <c r="R11" s="21"/>
+      <c r="S11" s="21"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A12" s="21"/>
+      <c r="B12" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="26">
+        <v>80015</v>
+      </c>
+      <c r="D12" s="21"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="21" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="21"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="21"/>
+      <c r="K12" s="21"/>
+      <c r="L12" s="21"/>
+      <c r="M12" s="21"/>
+      <c r="N12" s="21"/>
+      <c r="O12" s="21"/>
+      <c r="P12" s="21"/>
+      <c r="Q12" s="21"/>
+      <c r="R12" s="21"/>
+      <c r="S12" s="21"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A13" s="21"/>
+      <c r="B13" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C13" s="26">
+        <v>44601</v>
+      </c>
+      <c r="D13" s="21"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="21" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="21"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="21"/>
+      <c r="K13" s="21"/>
+      <c r="L13" s="21"/>
+      <c r="M13" s="21"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="21"/>
+      <c r="P13" s="21"/>
+      <c r="Q13" s="21"/>
+      <c r="R13" s="21"/>
+      <c r="S13" s="21"/>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A14" s="21"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="23"/>
+      <c r="D14" s="21"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="21"/>
+      <c r="G14" s="21"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="21"/>
+      <c r="K14" s="21"/>
+      <c r="L14" s="21"/>
+      <c r="M14" s="21"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="21"/>
+      <c r="P14" s="21"/>
+      <c r="Q14" s="21"/>
+      <c r="R14" s="21"/>
+      <c r="S14" s="21"/>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A15" s="21"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="14">
+        <v>64605</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="21"/>
+      <c r="F15" s="21"/>
+      <c r="G15" s="14">
+        <v>47495</v>
+      </c>
+      <c r="H15" s="14"/>
+      <c r="I15" s="14"/>
+      <c r="J15" s="21"/>
+      <c r="K15" s="21"/>
+      <c r="L15" s="21"/>
+      <c r="M15" s="21"/>
+      <c r="N15" s="21"/>
+      <c r="O15" s="21"/>
+      <c r="P15" s="21"/>
+      <c r="Q15" s="21"/>
+      <c r="R15" s="21"/>
+      <c r="S15" s="21"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A16" s="21"/>
+      <c r="B16" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="14">
+        <v>66125</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="21" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="14"/>
+      <c r="H16" s="14"/>
+      <c r="I16" s="14"/>
+      <c r="J16" s="21"/>
+      <c r="K16" s="21"/>
+      <c r="L16" s="21"/>
+      <c r="M16" s="21"/>
+      <c r="N16" s="21"/>
+      <c r="O16" s="21"/>
+      <c r="P16" s="21"/>
+      <c r="Q16" s="21"/>
+      <c r="R16" s="21"/>
+      <c r="S16" s="21"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A17" s="21"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="14">
+        <v>67657</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="21"/>
+      <c r="G17" s="14"/>
+      <c r="H17" s="14"/>
+      <c r="I17" s="14"/>
+      <c r="J17" s="21"/>
+      <c r="K17" s="21"/>
+      <c r="L17" s="21"/>
+      <c r="M17" s="21"/>
+      <c r="N17" s="21"/>
+      <c r="O17" s="21"/>
+      <c r="P17" s="21"/>
+      <c r="Q17" s="21"/>
+      <c r="R17" s="21"/>
+      <c r="S17" s="21"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A18" s="21"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="14">
+        <v>69140</v>
+      </c>
+      <c r="D18" s="21"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="21"/>
+      <c r="G18" s="14"/>
+      <c r="H18" s="14"/>
+      <c r="I18" s="14"/>
+      <c r="J18" s="21"/>
+      <c r="K18" s="21"/>
+      <c r="L18" s="21"/>
+      <c r="M18" s="21"/>
+      <c r="N18" s="21"/>
+      <c r="O18" s="21"/>
+      <c r="P18" s="21"/>
+      <c r="Q18" s="21"/>
+      <c r="R18" s="21"/>
+      <c r="S18" s="21"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A19" s="21"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="14">
+        <v>70684</v>
+      </c>
+      <c r="D19" s="21"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="21"/>
+      <c r="G19" s="14"/>
+      <c r="H19" s="14"/>
+      <c r="I19" s="14"/>
+      <c r="J19" s="21"/>
+      <c r="K19" s="21"/>
+      <c r="L19" s="21"/>
+      <c r="M19" s="21"/>
+      <c r="N19" s="21"/>
+      <c r="O19" s="21"/>
+      <c r="P19" s="21"/>
+      <c r="Q19" s="21"/>
+      <c r="R19" s="21"/>
+      <c r="S19" s="21"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A20" s="21"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="14">
+        <v>72204</v>
+      </c>
+      <c r="D20" s="21"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="21"/>
+      <c r="G20" s="14"/>
+      <c r="H20" s="14"/>
+      <c r="I20" s="14"/>
+      <c r="J20" s="21"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="21"/>
+      <c r="M20" s="21"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="21"/>
+      <c r="P20" s="21"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="21"/>
+      <c r="S20" s="21"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A21" s="21"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="14">
+        <v>73712</v>
+      </c>
+      <c r="D21" s="21"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="21"/>
+      <c r="G21" s="14"/>
+      <c r="H21" s="14"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="21"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="21"/>
+      <c r="M21" s="21"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="21"/>
+      <c r="P21" s="21"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="21"/>
+      <c r="S21" s="21"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A22" s="21"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="14">
+        <v>75244</v>
+      </c>
+      <c r="D22" s="21"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="21"/>
+      <c r="G22" s="14"/>
+      <c r="H22" s="14"/>
+      <c r="I22" s="14"/>
+      <c r="J22" s="21"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="21"/>
+      <c r="M22" s="21"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="21"/>
+      <c r="P22" s="21"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="21"/>
+      <c r="S22" s="21"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A23" s="21"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="14">
+        <v>76776</v>
+      </c>
+      <c r="D23" s="21"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="21"/>
+      <c r="G23" s="14">
+        <v>53809</v>
+      </c>
+      <c r="H23" s="14"/>
+      <c r="I23" s="14"/>
+      <c r="J23" s="21"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="21"/>
+      <c r="M23" s="21"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="21"/>
+      <c r="P23" s="21"/>
+      <c r="Q23" s="21"/>
+      <c r="R23" s="21"/>
+      <c r="S23" s="21"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A24" s="21"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
+      <c r="J24" s="21"/>
+      <c r="K24" s="21"/>
+      <c r="L24" s="21"/>
+      <c r="M24" s="21"/>
+      <c r="N24" s="21"/>
+      <c r="O24" s="21"/>
+      <c r="P24" s="21"/>
+      <c r="Q24" s="21"/>
+      <c r="R24" s="21"/>
+      <c r="S24" s="21"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A25" s="21"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="21"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A26" s="21"/>
+      <c r="B26" s="21"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="21"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
+      <c r="J26" s="21"/>
+      <c r="K26" s="21"/>
+      <c r="L26" s="21"/>
+      <c r="M26" s="21"/>
+      <c r="N26" s="21"/>
+      <c r="O26" s="21"/>
+      <c r="P26" s="21"/>
+      <c r="Q26" s="21"/>
+      <c r="R26" s="21"/>
+      <c r="S26" s="21"/>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A27" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="21"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="21"/>
+      <c r="G27" s="21"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
+      <c r="J27" s="21"/>
+      <c r="K27" s="21"/>
+      <c r="L27" s="21"/>
+      <c r="M27" s="21"/>
+      <c r="N27" s="21"/>
+      <c r="O27" s="21"/>
+      <c r="P27" s="21"/>
+      <c r="Q27" s="21"/>
+      <c r="R27" s="21"/>
+      <c r="S27" s="21"/>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A28" s="21"/>
+      <c r="B28" s="21"/>
+      <c r="C28" s="21"/>
+      <c r="D28" s="21"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
+      <c r="J28" s="21"/>
+      <c r="K28" s="21"/>
+      <c r="L28" s="21"/>
+      <c r="M28" s="21"/>
+      <c r="N28" s="21"/>
+      <c r="O28" s="21"/>
+      <c r="P28" s="21"/>
+      <c r="Q28" s="21"/>
+      <c r="R28" s="21"/>
+      <c r="S28" s="21"/>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A29" s="21"/>
+      <c r="B29" s="21"/>
+      <c r="C29" s="21"/>
+      <c r="D29" s="21"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
+      <c r="J29" s="21"/>
+      <c r="K29" s="21"/>
+      <c r="L29" s="21"/>
+      <c r="M29" s="21"/>
+      <c r="N29" s="21"/>
+      <c r="O29" s="21"/>
+      <c r="P29" s="21"/>
+      <c r="Q29" s="21"/>
+      <c r="R29" s="21"/>
+      <c r="S29" s="21"/>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A30" s="21"/>
+      <c r="B30" s="21"/>
+      <c r="C30" s="21"/>
+      <c r="D30" s="21"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
+      <c r="J30" s="21"/>
+      <c r="K30" s="21"/>
+      <c r="L30" s="21"/>
+      <c r="M30" s="21"/>
+      <c r="N30" s="21"/>
+      <c r="O30" s="21"/>
+      <c r="P30" s="21"/>
+      <c r="Q30" s="21"/>
+      <c r="R30" s="21"/>
+      <c r="S30" s="21"/>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A31" s="21"/>
+      <c r="B31" s="21"/>
+      <c r="C31" s="21"/>
+      <c r="D31" s="21"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
+      <c r="J31" s="21"/>
+      <c r="K31" s="21"/>
+      <c r="L31" s="21"/>
+      <c r="M31" s="21"/>
+      <c r="N31" s="21"/>
+      <c r="O31" s="21"/>
+      <c r="P31" s="21"/>
+      <c r="Q31" s="21"/>
+      <c r="R31" s="21"/>
+      <c r="S31" s="21"/>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A32" s="21"/>
+      <c r="B32" s="21"/>
+      <c r="C32" s="21"/>
+      <c r="D32" s="21"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
+      <c r="J32" s="21"/>
+      <c r="K32" s="21"/>
+      <c r="L32" s="21"/>
+      <c r="M32" s="21"/>
+      <c r="N32" s="21"/>
+      <c r="O32" s="21"/>
+      <c r="P32" s="21"/>
+      <c r="Q32" s="21"/>
+      <c r="R32" s="21"/>
+      <c r="S32" s="21"/>
+    </row>
+    <row r="33" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A33" s="21"/>
+      <c r="B33" s="21"/>
+      <c r="C33" s="21"/>
+      <c r="D33" s="21"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
+      <c r="J33" s="21"/>
+      <c r="K33" s="21"/>
+      <c r="L33" s="21"/>
+      <c r="M33" s="21"/>
+      <c r="N33" s="21"/>
+      <c r="O33" s="21"/>
+      <c r="P33" s="21"/>
+      <c r="Q33" s="21"/>
+      <c r="R33" s="21"/>
+      <c r="S33" s="21"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A34" s="21"/>
+      <c r="B34" s="21"/>
+      <c r="C34" s="21"/>
+      <c r="D34" s="21"/>
+      <c r="E34" s="21"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
+      <c r="J34" s="21"/>
+      <c r="K34" s="21"/>
+      <c r="L34" s="21"/>
+      <c r="M34" s="21"/>
+      <c r="N34" s="21"/>
+      <c r="O34" s="21"/>
+      <c r="P34" s="21"/>
+      <c r="Q34" s="21"/>
+      <c r="R34" s="21"/>
+      <c r="S34" s="21"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A35" s="21"/>
+      <c r="B35" s="21"/>
+      <c r="C35" s="21"/>
+      <c r="D35" s="21"/>
+      <c r="E35" s="21"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
+      <c r="J35" s="21"/>
+      <c r="K35" s="21"/>
+      <c r="L35" s="21"/>
+      <c r="M35" s="21"/>
+      <c r="N35" s="21"/>
+      <c r="O35" s="21"/>
+      <c r="P35" s="21"/>
+      <c r="Q35" s="21"/>
+      <c r="R35" s="21"/>
+      <c r="S35" s="21"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A36" s="21"/>
+      <c r="B36" s="21"/>
+      <c r="C36" s="21"/>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="21"/>
+      <c r="K36" s="21"/>
+      <c r="L36" s="21"/>
+      <c r="M36" s="21"/>
+      <c r="N36" s="21"/>
+      <c r="O36" s="21"/>
+      <c r="P36" s="21"/>
+      <c r="Q36" s="21"/>
+      <c r="R36" s="21"/>
+      <c r="S36" s="21"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A37" s="21"/>
+      <c r="B37" s="21"/>
+      <c r="C37" s="21"/>
+      <c r="D37" s="21"/>
+      <c r="E37" s="21"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
+      <c r="J37" s="21"/>
+      <c r="K37" s="21"/>
+      <c r="L37" s="21"/>
+      <c r="M37" s="21"/>
+      <c r="N37" s="21"/>
+      <c r="O37" s="21"/>
+      <c r="P37" s="21"/>
+      <c r="Q37" s="21"/>
+      <c r="R37" s="21"/>
+      <c r="S37" s="21"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A38" s="21"/>
+      <c r="B38" s="21"/>
+      <c r="C38" s="21"/>
+      <c r="D38" s="21"/>
+      <c r="E38" s="21"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
+      <c r="J38" s="21"/>
+      <c r="K38" s="21"/>
+      <c r="L38" s="21"/>
+      <c r="M38" s="21"/>
+      <c r="N38" s="21"/>
+      <c r="O38" s="21"/>
+      <c r="P38" s="21"/>
+      <c r="Q38" s="21"/>
+      <c r="R38" s="21"/>
+      <c r="S38" s="21"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A39" s="21"/>
+      <c r="B39" s="21"/>
+      <c r="C39" s="21"/>
+      <c r="D39" s="21"/>
+      <c r="E39" s="21"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="21"/>
+      <c r="J39" s="21"/>
+      <c r="K39" s="21"/>
+      <c r="L39" s="21"/>
+      <c r="M39" s="21"/>
+      <c r="N39" s="21"/>
+      <c r="O39" s="21"/>
+      <c r="P39" s="21"/>
+      <c r="Q39" s="21"/>
+      <c r="R39" s="21"/>
+      <c r="S39" s="21"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A40" s="21"/>
+      <c r="B40" s="21"/>
+      <c r="C40" s="21"/>
+      <c r="D40" s="21"/>
+      <c r="E40" s="21"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="21"/>
+      <c r="I40" s="21"/>
+      <c r="J40" s="21"/>
+      <c r="K40" s="21"/>
+      <c r="L40" s="21"/>
+      <c r="M40" s="21"/>
+      <c r="N40" s="21"/>
+      <c r="O40" s="21"/>
+      <c r="P40" s="21"/>
+      <c r="Q40" s="21"/>
+      <c r="R40" s="21"/>
+      <c r="S40" s="21"/>
+    </row>
+    <row r="41" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A41" s="21"/>
+      <c r="B41" s="21"/>
+      <c r="C41" s="21"/>
+      <c r="D41" s="21"/>
+      <c r="E41" s="21"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="21"/>
+      <c r="I41" s="21"/>
+      <c r="J41" s="21"/>
+      <c r="K41" s="21"/>
+      <c r="L41" s="21"/>
+      <c r="M41" s="21"/>
+      <c r="N41" s="21"/>
+      <c r="O41" s="21"/>
+      <c r="P41" s="21"/>
+      <c r="Q41" s="21"/>
+      <c r="R41" s="21"/>
+      <c r="S41" s="21"/>
+    </row>
+    <row r="42" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A42" s="21"/>
+      <c r="B42" s="21"/>
+      <c r="C42" s="21"/>
+      <c r="D42" s="21"/>
+      <c r="E42" s="21"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="21"/>
+      <c r="I42" s="21"/>
+      <c r="J42" s="21"/>
+      <c r="K42" s="21"/>
+      <c r="L42" s="21"/>
+      <c r="M42" s="21"/>
+      <c r="N42" s="21"/>
+      <c r="O42" s="21"/>
+      <c r="P42" s="21"/>
+      <c r="Q42" s="21"/>
+      <c r="R42" s="21"/>
+      <c r="S42" s="21"/>
+    </row>
+    <row r="43" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A43" s="21"/>
+      <c r="B43" s="21"/>
+      <c r="C43" s="21"/>
+      <c r="D43" s="21"/>
+      <c r="E43" s="21"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="21"/>
+      <c r="I43" s="21"/>
+      <c r="J43" s="21"/>
+      <c r="K43" s="21"/>
+      <c r="L43" s="21"/>
+      <c r="M43" s="21"/>
+      <c r="N43" s="21"/>
+      <c r="O43" s="21"/>
+      <c r="P43" s="21"/>
+      <c r="Q43" s="21"/>
+      <c r="R43" s="21"/>
+      <c r="S43" s="21"/>
+    </row>
+    <row r="44" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A44" s="21"/>
+      <c r="B44" s="21"/>
+      <c r="C44" s="21"/>
+      <c r="D44" s="21"/>
+      <c r="E44" s="21"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="21"/>
+      <c r="I44" s="21"/>
+      <c r="J44" s="21"/>
+      <c r="K44" s="21"/>
+      <c r="L44" s="21"/>
+      <c r="M44" s="21"/>
+      <c r="N44" s="21"/>
+      <c r="O44" s="21"/>
+      <c r="P44" s="21"/>
+      <c r="Q44" s="21"/>
+      <c r="R44" s="21"/>
+      <c r="S44" s="21"/>
+    </row>
+    <row r="45" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A45" s="21"/>
+      <c r="B45" s="21"/>
+      <c r="C45" s="21"/>
+      <c r="D45" s="21"/>
+      <c r="E45" s="21"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="21"/>
+      <c r="I45" s="21"/>
+      <c r="J45" s="21"/>
+      <c r="K45" s="21"/>
+      <c r="L45" s="21"/>
+      <c r="M45" s="21"/>
+      <c r="N45" s="21"/>
+      <c r="O45" s="21"/>
+      <c r="P45" s="21"/>
+      <c r="Q45" s="21"/>
+      <c r="R45" s="21"/>
+      <c r="S45" s="21"/>
+    </row>
+    <row r="46" spans="1:19" x14ac:dyDescent="0.35">
+      <c r="A46" s="21"/>
+      <c r="B46" s="21"/>
+      <c r="C46" s="21"/>
+      <c r="D46" s="21"/>
+      <c r="E46" s="21"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="21"/>
+      <c r="I46" s="21"/>
+      <c r="J46" s="21"/>
+      <c r="K46" s="21"/>
+      <c r="L46" s="21"/>
+      <c r="M46" s="21"/>
+      <c r="N46" s="21"/>
+      <c r="O46" s="21"/>
+      <c r="P46" s="21"/>
+      <c r="Q46" s="21"/>
+      <c r="R46" s="21"/>
+      <c r="S46" s="21"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B2:C3"/>
+    <mergeCell ref="F2:G3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>